<commit_message>
finished up the project files
</commit_message>
<xml_diff>
--- a/proj3_planning/results.xlsx
+++ b/proj3_planning/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="2580" windowWidth="14060" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="13120" yWindow="0" windowWidth="14060" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="13">
   <si>
     <t>Problem 1</t>
   </si>
@@ -51,7 +51,13 @@
     <t>depth_first_graph_search</t>
   </si>
   <si>
-    <t>astar_search</t>
+    <t>astar_search with h_1</t>
+  </si>
+  <si>
+    <t>astar_search with h_ignore_preconditions</t>
+  </si>
+  <si>
+    <t>astar_search with h_pg_levelsum</t>
   </si>
 </sst>
 </file>
@@ -100,8 +106,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -113,11 +147,39 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,15 +509,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1">
+        <v>1</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -495,7 +560,7 @@
         <v>180</v>
       </c>
       <c r="E3">
-        <v>3.0000831000506802E-2</v>
+        <v>7.8426908992696498E-2</v>
       </c>
       <c r="F3">
         <v>6</v>
@@ -515,7 +580,7 @@
         <v>30509</v>
       </c>
       <c r="E4">
-        <v>14.453282401001999</v>
+        <v>28.952266854001198</v>
       </c>
       <c r="F4">
         <v>9</v>
@@ -535,13 +600,16 @@
         <v>129631</v>
       </c>
       <c r="E5">
-        <v>98.272871554996499</v>
+        <v>182.17717483200201</v>
       </c>
       <c r="F5">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="A7">
+        <v>3</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -581,7 +649,7 @@
         <v>84</v>
       </c>
       <c r="E9">
-        <v>1.58216660056496E-2</v>
+        <v>2.6630198000930201E-2</v>
       </c>
       <c r="F9">
         <v>20</v>
@@ -601,7 +669,7 @@
         <v>5602</v>
       </c>
       <c r="E10">
-        <v>3.60701827400043</v>
+        <v>7.2162615499982996</v>
       </c>
       <c r="F10">
         <v>619</v>
@@ -621,16 +689,17 @@
         <v>3364</v>
       </c>
       <c r="E11">
-        <v>1.7274454729995301</v>
+        <v>3.1420503469998899</v>
       </c>
       <c r="F11">
         <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -667,7 +736,7 @@
         <v>224</v>
       </c>
       <c r="E15">
-        <v>3.5987076997116597E-2</v>
+        <v>6.8847660993924295E-2</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -687,7 +756,7 @@
         <v>44041</v>
       </c>
       <c r="E16">
-        <v>12.862359409999</v>
+        <v>22.126883590972199</v>
       </c>
       <c r="F16">
         <v>9</v>
@@ -701,23 +770,263 @@
         <v>18151</v>
       </c>
       <c r="C17">
-        <v>18151</v>
+        <v>18153</v>
       </c>
       <c r="D17">
         <v>159038</v>
       </c>
       <c r="E17">
-        <v>52.195040399004903</v>
+        <v>115.730096187005</v>
       </c>
       <c r="F17">
         <v>12</v>
       </c>
     </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>224</v>
+      </c>
+      <c r="E23">
+        <v>8.5609160014428198E-2</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>4853</v>
+      </c>
+      <c r="C24">
+        <v>4855</v>
+      </c>
+      <c r="D24">
+        <v>44041</v>
+      </c>
+      <c r="E24">
+        <v>20.296631225995899</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>18151</v>
+      </c>
+      <c r="C25">
+        <v>18153</v>
+      </c>
+      <c r="D25">
+        <v>159038</v>
+      </c>
+      <c r="E25">
+        <v>100.67678316100501</v>
+      </c>
+      <c r="F25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>41</v>
+      </c>
+      <c r="C31">
+        <v>43</v>
+      </c>
+      <c r="D31">
+        <v>170</v>
+      </c>
+      <c r="E31">
+        <v>6.7934118007542496E-2</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1450</v>
+      </c>
+      <c r="C32">
+        <v>1452</v>
+      </c>
+      <c r="D32">
+        <v>13303</v>
+      </c>
+      <c r="E32">
+        <v>7.9578909480187496</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>5038</v>
+      </c>
+      <c r="C33">
+        <v>5040</v>
+      </c>
+      <c r="D33">
+        <v>44926</v>
+      </c>
+      <c r="E33">
+        <v>32.798792346991803</v>
+      </c>
+      <c r="F33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0.31762763799633797</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B36:F36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>